<commit_message>
model overview page test setup
</commit_message>
<xml_diff>
--- a/Data Files/prodURLs.xlsx
+++ b/Data Files/prodURLs.xlsx
@@ -9,10 +9,30 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="allPages" sheetId="1" r:id="rId1"/>
+    <sheet name="miscPages" sheetId="15" r:id="rId2"/>
+    <sheet name="CategoryPages" sheetId="21" r:id="rId3"/>
+    <sheet name="ComparePages" sheetId="18" r:id="rId4"/>
+    <sheet name="DealerPages" sheetId="22" r:id="rId5"/>
+    <sheet name="FCVPages" sheetId="20" r:id="rId6"/>
+    <sheet name="HomeOffersPages" sheetId="19" r:id="rId7"/>
+    <sheet name="LCertifiedPages" sheetId="17" r:id="rId8"/>
+    <sheet name="SponsoredAthletes" sheetId="16" r:id="rId9"/>
+    <sheet name="ModelPagesOverview" sheetId="3" r:id="rId10"/>
+    <sheet name="ModelPagesGallery" sheetId="4" r:id="rId11"/>
+    <sheet name="ModelPagesFeatures" sheetId="5" r:id="rId12"/>
+    <sheet name="ModelPagesTechnology" sheetId="6" r:id="rId13"/>
+    <sheet name="ModelPagesPerformance" sheetId="7" r:id="rId14"/>
+    <sheet name="ModelPagesDesign" sheetId="8" r:id="rId15"/>
+    <sheet name="ModelPagesSafety" sheetId="9" r:id="rId16"/>
+    <sheet name="ModelPagesPackages" sheetId="10" r:id="rId17"/>
+    <sheet name="ModelPagesAccessories" sheetId="11" r:id="rId18"/>
+    <sheet name="ModelPagesSpecifications" sheetId="12" r:id="rId19"/>
+    <sheet name="ModelPagesOwners" sheetId="13" r:id="rId20"/>
+    <sheet name="ModelPagesOffers" sheetId="14" r:id="rId21"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="362">
   <si>
     <t>https://www.lexus.com</t>
   </si>
@@ -980,15 +1000,6 @@
     <t>https://www.lexus.com/motorsports</t>
   </si>
   <si>
-    <t>https://www.lexus.com/motorsports/#!about</t>
-  </si>
-  <si>
-    <t>https://www.lexus.com/motorsports/#team-team</t>
-  </si>
-  <si>
-    <t>https://www.lexus.com/motorsports/#races-events</t>
-  </si>
-  <si>
     <t>https://www.lexus.com/lexusplus</t>
   </si>
   <si>
@@ -1056,6 +1067,69 @@
   </si>
   <si>
     <t>https://www.lexus.com/request-newsletter</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/models/LC-convertible</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/models/IS/design</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/models/ES/design</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/models/GS/design</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/models/LS/design</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/models/UX/design</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/models/NX/design</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/models/RX/design</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/models/GX/design</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/models/LX/design</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/models/RC/design</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/models/RCF/design</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/models/LC/design</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/models/GSF/design</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/models/UX-hybrid/design</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/models/NX-hybrid/design</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/models/RX-hybrid/design</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/models/ES-hybrid/design</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/models/LC-hybrid/design</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/models/LS-hybrid/design</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/models/LC/technology</t>
   </si>
 </sst>
 </file>
@@ -1373,10 +1447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A348"/>
+  <dimension ref="A1:A365"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A343" workbookViewId="0">
-      <selection activeCell="B367" sqref="B367"/>
+    <sheetView topLeftCell="A325" workbookViewId="0">
+      <selection activeCell="A343" sqref="A343:XFD345"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,1622 +1577,3835 @@
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>341</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>81</v>
+        <v>361</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>107</v>
+        <v>342</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>108</v>
+        <v>343</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>109</v>
+        <v>344</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>110</v>
+        <v>345</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>111</v>
+        <v>346</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>112</v>
+        <v>347</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>113</v>
+        <v>348</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>114</v>
+        <v>349</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>115</v>
+        <v>350</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>116</v>
+        <v>351</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>117</v>
+        <v>352</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>118</v>
+        <v>353</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>119</v>
+        <v>354</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>120</v>
+        <v>355</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>121</v>
+        <v>356</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>122</v>
+        <v>357</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>123</v>
+        <v>358</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>124</v>
+        <v>359</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>125</v>
+        <v>360</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>254</v>
+        <v>234</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>255</v>
+        <v>235</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>265</v>
+        <v>245</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>268</v>
+        <v>249</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>269</v>
+        <v>250</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>270</v>
+        <v>251</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>271</v>
+        <v>252</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>272</v>
+        <v>253</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>273</v>
+        <v>254</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>274</v>
+        <v>255</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>275</v>
+        <v>256</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>276</v>
+        <v>257</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>277</v>
+        <v>258</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>278</v>
+        <v>259</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>279</v>
+        <v>260</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>280</v>
+        <v>261</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>282</v>
+        <v>263</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>283</v>
+        <v>264</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>284</v>
+        <v>265</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>285</v>
+        <v>266</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>287</v>
+        <v>268</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>288</v>
+        <v>269</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>290</v>
+        <v>271</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>293</v>
+        <v>275</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>295</v>
+        <v>277</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>296</v>
+        <v>278</v>
       </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>301</v>
+        <v>283</v>
       </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>302</v>
+        <v>284</v>
       </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>303</v>
+        <v>285</v>
       </c>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>304</v>
+        <v>286</v>
       </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>305</v>
+        <v>283</v>
       </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>306</v>
+        <v>287</v>
       </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>307</v>
+        <v>288</v>
       </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>308</v>
+        <v>289</v>
       </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>309</v>
+        <v>290</v>
       </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>310</v>
+        <v>267</v>
       </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>311</v>
+        <v>291</v>
       </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>313</v>
+        <v>293</v>
       </c>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>315</v>
+        <v>295</v>
       </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>316</v>
+        <v>296</v>
       </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>317</v>
+        <v>297</v>
       </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>320</v>
+        <v>300</v>
       </c>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>321</v>
+        <v>301</v>
       </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>324</v>
+        <v>304</v>
       </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>325</v>
+        <v>305</v>
       </c>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>326</v>
+        <v>306</v>
       </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>331</v>
+        <v>311</v>
       </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>332</v>
+        <v>312</v>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>333</v>
+        <v>313</v>
       </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>334</v>
+        <v>314</v>
       </c>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>335</v>
+        <v>315</v>
       </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>336</v>
+        <v>316</v>
       </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>337</v>
+        <v>317</v>
       </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>338</v>
+        <v>318</v>
       </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>340</v>
+        <v>320</v>
       </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>341</v>
+        <v>321</v>
       </c>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>342</v>
+        <v>322</v>
       </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>340</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A25" r:id="rId1"/>
+    <hyperlink ref="A82" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A13" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD190"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A12" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD171"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>343</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD95"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD76"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>340</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>238</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>258</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>267</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tests created for all page categories
</commit_message>
<xml_diff>
--- a/Data Files/prodURLs.xlsx
+++ b/Data Files/prodURLs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="allPages" sheetId="1" r:id="rId1"/>
@@ -17,22 +17,23 @@
     <sheet name="CategoryPages" sheetId="21" r:id="rId3"/>
     <sheet name="ComparePages" sheetId="18" r:id="rId4"/>
     <sheet name="DealerPages" sheetId="22" r:id="rId5"/>
-    <sheet name="FCVPages" sheetId="20" r:id="rId6"/>
-    <sheet name="HomeOffersPages" sheetId="19" r:id="rId7"/>
-    <sheet name="LCertifiedPages" sheetId="17" r:id="rId8"/>
-    <sheet name="SponsoredAthletes" sheetId="16" r:id="rId9"/>
-    <sheet name="ModelPagesOverview" sheetId="3" r:id="rId10"/>
-    <sheet name="ModelPagesGallery" sheetId="4" r:id="rId11"/>
-    <sheet name="ModelPagesFeatures" sheetId="5" r:id="rId12"/>
-    <sheet name="ModelPagesTechnology" sheetId="6" r:id="rId13"/>
-    <sheet name="ModelPagesPerformance" sheetId="7" r:id="rId14"/>
-    <sheet name="ModelPagesDesign" sheetId="8" r:id="rId15"/>
-    <sheet name="ModelPagesSafety" sheetId="9" r:id="rId16"/>
-    <sheet name="ModelPagesPackages" sheetId="10" r:id="rId17"/>
-    <sheet name="ModelPagesAccessories" sheetId="11" r:id="rId18"/>
-    <sheet name="ModelPagesSpecifications" sheetId="12" r:id="rId19"/>
-    <sheet name="ModelPagesOwners" sheetId="13" r:id="rId20"/>
-    <sheet name="ModelPagesOffers" sheetId="14" r:id="rId21"/>
+    <sheet name="ErrorPages" sheetId="23" r:id="rId6"/>
+    <sheet name="FCVPages" sheetId="20" r:id="rId7"/>
+    <sheet name="HomeOffersPages" sheetId="19" r:id="rId8"/>
+    <sheet name="LCertifiedPages" sheetId="17" r:id="rId9"/>
+    <sheet name="SponsoredAthletes" sheetId="16" r:id="rId10"/>
+    <sheet name="ModelPagesOverview" sheetId="3" r:id="rId11"/>
+    <sheet name="ModelPagesGallery" sheetId="4" r:id="rId12"/>
+    <sheet name="ModelPagesFeatures" sheetId="5" r:id="rId13"/>
+    <sheet name="ModelPagesTechnology" sheetId="6" r:id="rId14"/>
+    <sheet name="ModelPagesPerformance" sheetId="7" r:id="rId15"/>
+    <sheet name="ModelPagesDesign" sheetId="8" r:id="rId16"/>
+    <sheet name="ModelPagesSafety" sheetId="9" r:id="rId17"/>
+    <sheet name="ModelPagesPackages" sheetId="10" r:id="rId18"/>
+    <sheet name="ModelPagesAccessories" sheetId="11" r:id="rId19"/>
+    <sheet name="ModelPagesSpecifications" sheetId="12" r:id="rId20"/>
+    <sheet name="ModelPagesOwners" sheetId="13" r:id="rId21"/>
+    <sheet name="ModelPagesOffers" sheetId="14" r:id="rId22"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="364">
   <si>
     <t>https://www.lexus.com</t>
   </si>
@@ -1130,6 +1131,12 @@
   </si>
   <si>
     <t>https://www.lexus.com/models/LC/technology</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/sfddsf</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/$#@$</t>
   </si>
 </sst>
 </file>
@@ -3292,6 +3299,87 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>332</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
@@ -3408,7 +3496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A19"/>
   <sheetViews>
@@ -3518,7 +3606,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A19"/>
   <sheetViews>
@@ -3628,7 +3716,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A19"/>
   <sheetViews>
@@ -3741,7 +3829,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A19"/>
   <sheetViews>
@@ -3851,7 +3939,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A38"/>
   <sheetViews>
@@ -4056,7 +4144,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A19"/>
   <sheetViews>
@@ -4166,7 +4254,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A19"/>
   <sheetViews>
@@ -4276,7 +4364,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A19"/>
   <sheetViews>
@@ -4379,116 +4467,6 @@
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>181</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD57"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -4667,6 +4645,116 @@
   <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20:XFD38"/>
     </sheetView>
   </sheetViews>
@@ -4772,7 +4860,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A19"/>
   <sheetViews>
@@ -4886,7 +4974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD43"/>
     </sheetView>
   </sheetViews>
@@ -5087,6 +5175,36 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2" location="@$"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5131,7 +5249,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
@@ -5172,7 +5290,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A29"/>
   <sheetViews>
@@ -5331,85 +5449,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>332</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added SSO authentication for FCV tests
</commit_message>
<xml_diff>
--- a/Data Files/prodURLs.xlsx
+++ b/Data Files/prodURLs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="allPages" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="367">
   <si>
     <t>https://www.lexus.com</t>
   </si>
@@ -1137,6 +1137,15 @@
   </si>
   <si>
     <t>https://www.lexus.com/$#@$</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/dealers/60419-keyes-lexus</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/dealers/60406-lexus-santa-monica</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/dealers/60445-lexus-of-cerritos</t>
   </si>
 </sst>
 </file>
@@ -4953,7 +4962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -5117,10 +5126,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5150,9 +5159,29 @@
         <v>295</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A6" r:id="rId1"/>
+    <hyperlink ref="A7" r:id="rId2"/>
+    <hyperlink ref="A8" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
debugged fcv nav check, open browser loop that was causing duplicates
</commit_message>
<xml_diff>
--- a/Data Files/prodURLs.xlsx
+++ b/Data Files/prodURLs.xlsx
@@ -1139,13 +1139,13 @@
     <t>https://www.lexus.com/$#@$</t>
   </si>
   <si>
-    <t>https://www.lexus.com/dealers/60419-keyes-lexus</t>
-  </si>
-  <si>
     <t>https://www.lexus.com/dealers/60406-lexus-santa-monica</t>
   </si>
   <si>
     <t>https://www.lexus.com/dealers/60445-lexus-of-cerritos</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/dealers/60409-keyes-lexus</t>
   </si>
 </sst>
 </file>
@@ -5129,7 +5129,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5161,17 +5161,17 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated to check all misc pages for IE11 message, even if one is missing
</commit_message>
<xml_diff>
--- a/Data Files/prodURLs.xlsx
+++ b/Data Files/prodURLs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="allPages" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="367">
   <si>
     <t>https://www.lexus.com</t>
   </si>
@@ -1480,1829 +1480,1829 @@
       <selection activeCell="A343" sqref="A343:XFD345"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A176" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A179" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A180" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A181" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A182" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A183" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A184" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A185" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A186" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A188" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A189" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A190" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A191" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A192" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A193" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A194" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A196" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A199" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A200" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A203" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A204" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A205" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A206" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A207" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A208" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A209" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A210" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A211" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A212" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A213" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A214" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A215" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A216" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A217" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A218" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A219" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A220" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A221" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A222" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A223" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A224" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A225" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A226" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A227" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A228" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A229" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A230" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A231" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A232" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A233" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A234" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A235" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A236" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A237" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A238" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A239" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A240" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A241" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A242" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A243" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A244" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A245" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A246" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A247" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A248" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A249" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A250" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A251" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A252" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A253" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A254" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A255" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A256" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A257" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A258" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A259" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A260" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A261" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A262" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A263" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A264" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A265" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A266" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A267" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A268" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A269" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A270" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A271" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A272" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A273" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A274" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A275" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A276" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A277" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A278" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A279" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A280" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A281" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A282" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A283" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A284" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A285" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A286" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A287" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A288" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A289" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A290" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A291" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A292" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A293" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A294" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A295" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A296" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A297" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A298" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A299" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A300" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A301" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A302" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A303" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A304" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A305" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A306" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A307" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A308" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A309" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A310" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A311" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A312" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A313" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A314" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A315" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A316" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A317" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A318" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A319" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A320" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A321" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A322" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A323" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A324" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A325" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A326" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A327" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A328" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A329" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A330" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A331" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A332" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A333" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A334" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A335" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A336" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A337" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A338" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A339" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A340" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A341" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A342" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A343" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A344" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A345" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A346" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A347" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A348" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A349" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A350" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A351" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A352" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A353" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A354" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A355" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A356" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A357" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A358" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A359" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A360" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A361" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A362" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A363" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A364" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A365" t="s">
         <v>340</v>
       </c>
@@ -3325,69 +3325,69 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>332</v>
       </c>
@@ -3406,104 +3406,104 @@
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -3524,99 +3524,99 @@
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -3634,99 +3634,99 @@
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>68</v>
       </c>
@@ -3744,99 +3744,99 @@
       <selection activeCell="A20" sqref="A20:XFD190"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>87</v>
       </c>
@@ -3857,99 +3857,99 @@
       <selection activeCell="A20" sqref="A20:XFD171"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>105</v>
       </c>
@@ -3967,149 +3967,149 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>124</v>
       </c>
@@ -4133,99 +4133,99 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>143</v>
       </c>
@@ -4243,99 +4243,99 @@
       <selection activeCell="A20" sqref="A20:XFD95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>162</v>
       </c>
@@ -4353,99 +4353,99 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>181</v>
       </c>
@@ -4467,154 +4467,154 @@
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>340</v>
       </c>
@@ -4636,99 +4636,99 @@
       <selection activeCell="A20" sqref="A20:XFD57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>200</v>
       </c>
@@ -4746,99 +4746,99 @@
       <selection activeCell="A20" sqref="A20:XFD38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>219</v>
       </c>
@@ -4856,99 +4856,99 @@
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>238</v>
       </c>
@@ -4966,34 +4966,34 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -5010,111 +5010,101 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
         <v>258</v>
       </c>
     </row>
@@ -5128,48 +5118,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>365</v>
       </c>
@@ -5191,14 +5181,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>363</v>
       </c>
@@ -5221,34 +5211,34 @@
       <selection activeCell="A7" sqref="A7:XFD46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>264</v>
       </c>
@@ -5267,29 +5257,29 @@
       <selection activeCell="A6" sqref="A6:XFD51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -5308,149 +5298,149 @@
       <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>267</v>
       </c>

</xml_diff>

<commit_message>
added check for page title meta
</commit_message>
<xml_diff>
--- a/Data Files/prodURLs.xlsx
+++ b/Data Files/prodURLs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="allPages" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="370">
   <si>
     <t>https://www.lexus.com</t>
   </si>
@@ -1146,6 +1146,15 @@
   </si>
   <si>
     <t>https://www.lexus.com/dealers/60409-keyes-lexus</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/enform/</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/enform/in-dash-technology/</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/enform/availability-pricing/</t>
   </si>
 </sst>
 </file>
@@ -4461,10 +4470,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A30"/>
+  <dimension ref="A1:A34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4535,96 +4544,118 @@
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
         <v>310</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>314</v>
+      <c r="A18" s="1" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>315</v>
+      <c r="A19" s="1" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
         <v>340</v>
       </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A34" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A24" r:id="rId1"/>
+    <hyperlink ref="A27" r:id="rId1"/>
+    <hyperlink ref="A15" r:id="rId2"/>
+    <hyperlink ref="A14" r:id="rId3"/>
+    <hyperlink ref="A18" r:id="rId4"/>
+    <hyperlink ref="A19" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -5012,7 +5043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
staging model page tests added with updated cepo URLs
</commit_message>
<xml_diff>
--- a/Data Files/prodURLs.xlsx
+++ b/Data Files/prodURLs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="allPages" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="372">
   <si>
     <t>https://www.lexus.com</t>
   </si>
@@ -1155,6 +1155,12 @@
   </si>
   <si>
     <t>https://www.lexus.com/enform/availability-pricing/</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/IS500/</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/LF-Z-Electrified/</t>
   </si>
 </sst>
 </file>
@@ -4472,7 +4478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
@@ -5233,17 +5239,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>259</v>
+        <v>370</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
@@ -5253,22 +5259,27 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>264</v>
+        <v>371</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>